<commit_message>
Added references, optimized news and graphs
</commit_message>
<xml_diff>
--- a/assets/text.xlsx
+++ b/assets/text.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shiny.cucumber\projects\ukraine_data\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7ACBBF4-4338-4A45-BFAE-40FFB8DDDC54}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC036F9D-33A0-4404-854D-C6D284FDC03C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="22140" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="2088" windowWidth="21924" windowHeight="10296" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -22,114 +22,80 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="36">
-  <si>
-    <t>Aside from energy, the fallout via trade for the rest of Europe is likely to be small. Non-energy trade and investment links between Russia and many European countries have declined in importance since 2013, with partial decoupling as a result of the exchange of sanctions following the annexation of Crimea. The most significant links are in CESEE; but even there, with a couple of exceptions, non-energy reliance on Russia is very limited. Even in a scenario where Russian demand falls by 10%, imports by 30% and exports by 13%, the negative hit to GDP growth in the rest of Europe via the trade channel (excluding energy) would be at most -0.25%, with the worst-affected countries mostly in CESEE. Using the ‘partial global extraction method’ to get a perhaps more realistic scenario, with adjustment via substitution, the impact on GDP in the rest of Europe would be even smaller.</t>
-  </si>
-  <si>
-    <t>If the EU were to ban imports of energy from Russia, or if Russia itself limits or stops gas exports to the EU, the trade impacts would be much more significant. More far-reaching moves to restrict or halt imports of Russian oil and gas by the EU are no longer inconceivable. As the Russian armed forces turn increasingly to indiscriminate shelling of civilian areas, and with allegations of war crimes by Russian forces starting to emerge, public anger in the rest of Europe will only grow, and there will be increased political space for EU leaders to take the undoubtedly economically painful step of cutting off Russian energy revenues.</t>
-  </si>
-  <si>
-    <t>The ‘temporary protection’ scheme introduced by the European Commission is an unambiguously positive step to foster Ukrainian refugees’ integration into EU labour markets. However, there are several major challenges. First, those fleeing the war are mostly women, children and the elderly. Second, some EU labour markets are still recovering from the COVID-19 crisis. Third, although the average education level of Ukrainians is above the EU average, there are some doubts about the transferability of refugees’ skills, knowledge and work experience, at least in the short-run.</t>
-  </si>
-  <si>
-    <t>Financial contagion is already visible in CESEE: currencies have weakened in countries near to Russia and Ukraine due to higher risk aversion, and interest rates on government debt have increased in some cases. Investor sentiment – both domestic and foreign – in the Baltic states is likely to suffer amid fears that Russia has designs on more than Ukraine. Nevertheless, most of the region has strong macroeconomic fundamentals, and policymakers have some space to use fiscal and monetary tools to ensure macro-financial stability.</t>
-  </si>
-  <si>
-    <t>The medium- and long-term outlook for Ukraine, Russia and the rest of Europe has been changed radically by the events of the last few weeks. For Ukraine, if one part of the country is occupied and the other part remains independent, economic outcomes will be very divergent. An independent part of Ukraine would see many refugees return, would receive massive Western financial support and could look forward to greater integration with the EU. Western investment would drive technological upgrading and productivity improvements. The IT sector – already advanced – would develop further. And the agricultural sector, where land reform was implemented recently, has great potential for increases in efficiency, which could be brought about by increased post-war investment. By contrast, a Russian-occupied East Ukraine would be rebuilt much more slowly, would continue to suffer from outward migration and would form part of a Russia-dominated world that has become relatively isolated from the global economy (except for its links with China – links that are unlikely to be very important for these regions of Ukraine).</t>
-  </si>
-  <si>
-    <t>For Russia, the medium-term outlook is largely negative. The sanctions mean that the economy will lose its access to Western technological transfer, which will increase its economic backwardness relative to the rest of the world. This will be partly – but far from completely – offset by rising integration with the major Asian economies, especially China. Real incomes are likely to stagnate. The Russian invasion also looks set to presage a fundamental unwinding of 30 years of economic integration between Russia and the West. On top of the harsh financial sanctions imposed on Russia, Western firms are leaving Russia en masse. That creates the likelihood that, even if at some point sanctions are eased, February 2022 may well prove to have been the swansong for European economic integration in its broadest sense.</t>
-  </si>
-  <si>
-    <t>There are four main areas of structural change and lasting impact for the EU (and Europe more broadly) as a result of Russia’s invasion of Ukraine. First, the EU will get more serious about defence. Second, the green transition will gather pace. Third, broader Eurasian economic integration will be unwound. And fourth, the EU accession prospects for countries in Southeast Europe could (and should) improve.</t>
-  </si>
-  <si>
-    <t>Western policymakers have a lengthy to-do list in the short term. The immediate priority must be to address the humanitarian crisis, including supporting and integrating refugees, providing assistance where possible for internally displaced people within Ukraine, and helping those countries where most refugees are arriving (such as Poland and Moldova). The next step is to address integration, including language training and active labour market policies to ease job access. Once the war ends, the US and EU should be ready with a plan for reconstruction, including identifying the most urgent areas where support will be needed (transport, housing, administration, etc.). They should also determine the scale and sequencing of this support, and encourage a significant return flow of refugees, once this becomes feasible. Technical assistance to the government will be crucial in rebuilding the economy from its war mode and advancing with reforms. The EU should make specific efforts to integrate post-war Ukraine much more strongly. This should include participation in all major EU programmes, just as if the country were an EU member: the cohesion funds, exchange programmes, research and scientific cooperation, trans-European transport and other infrastructure projects, common energy policy and programmes linked to the New Green Deal.</t>
-  </si>
-  <si>
-    <t>The Russian invasion of Ukraine has triggered a humanitarian crisis. Urban warfare is causing massive damage to critical civilian infrastructure, and there is a high risk of starvation, infection, and a rapid deterioration in people’s physical and mental health. Pre-war, almost 19m people lived in those regions that are currently directly affected. Refugee inflows to the rest of Europe are likely to be at least three times greater than in 2015/2016.</t>
-  </si>
-  <si>
-    <t>As a result of the war and the sanctions, the rest of Europe faces a surge in already high inflation; this will weigh on real incomes and could depress economic growth. In Germany, we estimate that each doubling of the gas price causes GDP to decline by over 1 percentage point. Many European countries rely heavily on Russia for oil and gas imports: import shares are over 75% in Czechia, Latvia, Hungary, Slovakia and Bulgaria with respect to natural gas; Slovakia, Lithuania, Poland and Finland with respect to oil and petroleum; and Cyprus, Estonia, Latvia, Denmark, Lithuania, Greece and Bulgaria with respect to solid fuels.</t>
-  </si>
-  <si>
-    <t>The economic costs of the invasion in Ukraine will be profound. Available estimates put the damage and destruction of physical infrastructure so far at USD 62.6bn. However, the cost of making good those losses is likely to be much higher. The regions of Ukraine that are currently directly affected by the conflict account for 53% of GDP. About one third of industrial and agricultural production, and about a quarter of exports originate in the conflict regions (excluding Kyiv city). Economic activity has practically ceased in the affected regions. With the Black Sea ports being blocked, Ukraine has lost its ability to sell more than half of its exports, primarily agricultural commodities and metals. Merchandise exports accounted for more than a third of the country’s GDP in 2021.</t>
-  </si>
-  <si>
-    <t>The Ukrainian economy so far has shown remarkable macro-financial resilience. However, this may change as many companies stop functioning and as unemployment rises. Banks will face substantial losses, due to the damage caused to their physical assets and the high probability of defaults on many loans. Western financial support will become ever more important as the war continues.</t>
-  </si>
-  <si>
-    <t>key_damage</t>
-  </si>
-  <si>
-    <t>ukraine_costs</t>
-  </si>
-  <si>
-    <t>ukraine_macro</t>
-  </si>
-  <si>
-    <t>russia_economy</t>
-  </si>
-  <si>
-    <t>europe_inflation</t>
-  </si>
-  <si>
-    <t>europe_trade_exposure</t>
-  </si>
-  <si>
-    <t>europe_energy</t>
-  </si>
-  <si>
-    <t>europe_finance</t>
-  </si>
-  <si>
-    <t>outlook_ukraine</t>
-  </si>
-  <si>
-    <t>outlook_russia</t>
-  </si>
-  <si>
-    <t>outlook_eu</t>
-  </si>
-  <si>
-    <t>russia_policies</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Turning to Russia, sanctions will have a very serious impact on that country’s economy and financial sector. wiiw estimate that Russian GDP will contract by at least 7-8% this year and inflation will accelerate to close to 30% by the end of 2022. During the first week of the crisis, Russia faced capital flight, FX depreciation and deposit outflows. However, the range of estimates in the economists' community is broad with some analysts predicting the GDP contraction by 15% within a year. </t>
-  </si>
-  <si>
-    <t>Despite being partly hamstrung by the fact that a large proportion of Russian reserve assets are frozen in the EU and G7, the central bank managed to stabilise financial markets by a combination of confidence-building and hard-steering measures: capital controls, FX controls, regulatory easing for financial institutions, and a doubling of the key policy rate. Although these measures were effective in curtailing financial panic, they further undermined investor confidence and increased the costs of borrowing for business. The fiscal stimulus so far announced is very limited, especially considering the likely scale of the contraction, and is not going to offset a sharp decline in real household incomes in 2022.</t>
-  </si>
-  <si>
-    <t>europe_refugees</t>
-  </si>
-  <si>
-    <t>policies</t>
-  </si>
-  <si>
-    <t>russia_sanctions</t>
-  </si>
-  <si>
-    <t>There are several caveats surrounding the sanctions' impact. First, quantity is not quality. Most of the sanctions impose restrictions on individuals and have a limited impact on the aggregate economy. Most importantly, the EU has still not imposed an energy embargo, which would have the biggest impact on the Russian fiscal position. Second, it is impossible to effectively impose sanctions exclusively against elites, without harming the general population. Sector-wide sanctions will cause hardship for ordinary Russians, but even individual-related sanctions do not avoid collateral damage. Evidence from Russia and other countries suggests that governments are likely to compensate the elites for their losses at the expense of taxpayers. There is a high chance that campaigns to boycott all Russian public institutions, together with the exodus of Western franchises from the Russian market, will affect mainly well-educated Russians living in big cities – those very people who value individuality over grand political achievements, who deliver and consume diverse media content, and who are most critical of the Putin regime. With their income opportunities and information flows constrained, they will become more dependent on state-provided revenues. This, in turn, will increase the likelihood that they are co-opted and that the anti-Western sentiment in Russia will harden.</t>
-  </si>
-  <si>
-    <t>summary_long_effects</t>
-  </si>
-  <si>
-    <t>summary_short_effects</t>
-  </si>
-  <si>
-    <t>The Russian invasion of Ukraine has triggered a humanitarian, economic, financial and political crisis that will reverberate across Europe. Much of Ukraine is already devastated by the war, with around 19m people and over half of the country’s GDP in the regions currently directly affected. Meanwhile we estimate that Russian GDP will contract by 7-8% this year, and inflation will accelerate to close to 30% by the end of 2022. For the rest of Europe, the impact will be felt via various channels, with the most significant so far being inflation on the back of high energy prices. If the EU were to ban imports of energy from Russia, or if Russia itself limits or stops gas exports to the EU, the trade impacts would be much more significant.</t>
-  </si>
-  <si>
-    <t>The medium- and long-term outlook for Ukraine, Russia and the rest of Europe has been changed radically by the events of the last few weeks. For Ukraine, if one part of the country is occupied and the other part remains independent, economic outcomes will be very divergent, but the non-occupied part would see many refugees return, would receive massive Western financial support and could look forward to greater integration with the EU. For Russia, the economy will lose its access to Western technological transfer, and this cannot be fully compensated by China; an already meagre medium-term growth outlook has now deteriorated further. Meanwhile there are four main areas of structural change and lasting impact for the EU and Europe more broadly: the EU will get more serious about defence, the green transition will gather pace, broader Eurasian economic integration will be unwound, and the EU accession prospects for countries in Southeast Europe could (and should) improve.</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
   <si>
     <t>text</t>
   </si>
   <si>
     <t>title</t>
+  </si>
+  <si>
+    <t>Casualties</t>
+  </si>
+  <si>
+    <t>Displacement</t>
+  </si>
+  <si>
+    <t>Monetary sector</t>
+  </si>
+  <si>
+    <t>War presents a challenge for financial stability of Ukraine due to increased military expenditures, increased volatility on financial markets, and disruption of operations of the war-affected areas. Inflation - especially for the basic consumer goods - remains the largest challenge for the monetary authorities, which is hard to curtail due to emission financing of the government budget. The FX rate is effectively fixed by the National Bank of Ukraine, yet it comes at cost of capital controls and requirements for international reserves.</t>
+  </si>
+  <si>
+    <t>National bank tools</t>
+  </si>
+  <si>
+    <t>Financial system</t>
+  </si>
+  <si>
+    <t>Ukraine's financial system remained stable during the crisis. During the onset of war, banks' profitability and liquidity remained similar to the pre-war levels. Latest data show increasing share of non-peforming loans, which follows the disruption of business operations due to continuing attacks of the Russian troops by on civilian objects and a mid-year interest rate increase.</t>
+  </si>
+  <si>
+    <t>Government finance</t>
+  </si>
+  <si>
+    <t>Ukraine support</t>
+  </si>
+  <si>
+    <t>Grain deal</t>
+  </si>
+  <si>
+    <t>War and reconstruction</t>
+  </si>
+  <si>
+    <t>Conflict intensity</t>
+  </si>
+  <si>
+    <t>The Russian invasion of Ukraine has triggered a humanitarian, economic, financial and political crisis with adverse impact on global security. Much of Ukraine is devastated by the war, with around half of Ukraine's population being displaced for almost a year. Urban warfare and deliberate attacks by the Russian troops the on Ukrainian infrastructure prolong the humanitarian crisis increasing risks of starvation, infection, and a rapid deterioration in people’s physical and mental health on a mass scale. The dashboard provides an overview of the key metrics related to war's impact on humanitarian issues, macroeconomic imbalances, and international support to Ukraine. The dashboard is assembled using third party data available publicly. Data are updated on the daily basis.</t>
+  </si>
+  <si>
+    <t>Summary</t>
+  </si>
+  <si>
+    <t>The number of conflict events is uncertain and is estimated based on the media reports collected and processed by the ACLED team. That being said any hostilities unreported by media might have remained unaccounted in the dataset. Follow the [ACLED website](https://acleddata.com/download/35224/) for more details on the methodology of the data collection process. For a comprehensive overview of the conflict events in Ukraine, follow the [ACLED's dedicated page](https://acleddata.com/ukraine-crisis/)</t>
+  </si>
+  <si>
+    <t>Russian invasion made millions of Ukrainians flee from the war both by moving inside Ukraine (internal displacement) and moving abroad (refugees). All reported data on migration face uncertainty. Refugee data may from suffer double-counting with the same person being reported as a refugee in multiple countries (see [UNHCR](https://data.unhcr.org/en/situations/ukraine) for background information). The number of internally displaced persons are survey-based estimates conducted by the International Organisation for Migration, which are scaled up to the size of the whole population. See the [IOM dashboard](https://displacement.iom.int/ukraine) for more information on the survey methodology.</t>
+  </si>
+  <si>
+    <t>Shortly after the start of the war, National Bank of Ukraine introduced administrative regulation of the capital markets by fixing the exchange rate and restricting capital flows outside of Ukraine. Under this setup, the volume of available foreign exchange reserves is among the key metrics to follow as it assures stability of the FX rate. Due limited possibilities of export and a heavy contraction of economy, Ukraine heavily relies on external lending for continuing inflow of foreign currency. See the [NBU review of inflation and monetary policy](https://bank.gov.ua/en/monetary) for more details.</t>
+  </si>
+  <si>
+    <t>With the onset of war, Ukraine's government massively increased expenditures to increase defence spending and support essential services for displaced persons. Defence spending accounts for around 40% of the total government expenditure and is roughly equivalent to the size of fiscal deficit run by the government. Ministry of finance expects fiscal deficit to be at the level of 20% of GDP in 2023, which will be financed by emission financing, external borrowing, and internal bond placements. Note that displaced figures depict monthly-run income and expenditures in national currency (UAH).</t>
+  </si>
+  <si>
+    <t>EU and G7 countries were quick in publicly announcing their support to Ukraine. Media-sourced data collected by [IFW Kiel](https://www.ifw-kiel.de/topics/war-against-ukraine/ukraine-support-tracker/) - a German-based think-tank on international economy shows that delivered amounts are behind the publicy announced promises: only 13% as of January 2023. US remains the key supporter of Ukraine in absolute volumes with a "delivery rate" of about 10%. Poland and the Baltic states remain the key supporters in relative numbers. Most of the delivered support was for the Ukrainian military.</t>
+  </si>
+  <si>
+    <t>The grain deal arranged between Ukraine, Russia, and Türkiye helped to ease tension on the global market for agriculture. The majority of the shipments was transferred to high- and upper middle-income countries with China, Spain, Türkiye, Italy, and Netherlands being the primary recepients (63% of total amount). The deal lasts for 120 days and extends automatically unless one of the parties declare to leave the deal. The next deal extension is expected on March 19th, 2023. Follow the [UN Joint Coordination Centre](https://www.un.org/en/black-sea-grain-initiative/updates) for the background information.</t>
+  </si>
+  <si>
+    <t>Data for reconstruction show estimates as of August 2022 reported by the [World Bank Rapid Damage and Needs Assessment](https://documents1.worldbank.org/en/publication/documents-reports/documentdetail/099445209072239810). Damage data were assessed using a mixture of bottom-up (surveys and on-site visits) and top-down assessments (satellite imagery, evaluations of authorities). The data does not include damage and corresponding needs caused by hostilities starting from September 2022 and does not include progress of the restoration activities already taking place in the regained territories of Ukraine. The scale of damage will require a decade-long process. As reconstruction needs exceed the pre-war Ukrainian GDP, the reconstruction process will require external finance.</t>
+  </si>
+  <si>
+    <t>The officially reported number of civilian casualties is reported by the Office of the High Commissioner for Human Rights (OHCHR). These numbers - as [acknowledged by OHCHR](https://www.ohchr.org/en/news/2023/01/ukraine-civilian-casualty-update-10-january-2023) remain considerably below the true value because '*information from some locations where intense hostilities have been going on has been delayed and many reports are still pending corroboration. This concerns, for example, Mariupol (Donetsk region), Izium (Kharkiv region), Lysychansk, Popasna, and Sievierodonetsk (Luhansk region), where there are allegations of numerous civilian casualties.*'
+The alternative number of casualties ('Fatalities') is based on media-based data sourced by ACLED. This estimation is effectively based on witnesses' evidence and does not have official confirmation from authorities (e.g. in the form of death certificates).
+The number of casualties on the territories under control by the Russian armed forces remain the largest source of concern. The largest uncertainty surrounds the city of Mariupol, which experienced a humanitarian catastrophe during the siege by the Russian Armed Forces in Spring 2022. Estimates of unaccounted deaths in Mariupol vary greatly. [Associated press estimated](https://apnews.com/article/russia-ukraine-war-erasing-mariupol-methodology-f74b28016b8dea4b82811655f14931f2?utm_source=apnews&amp;utm_medium=relatedcontentmodule) at least 10 000 dead persons in Mariupol based on the satellite imagery of graves at the city cemetry. Ukrainian officials - as [reported by BBC](https://www.bbc.com/news/world-europe-63536564) - suggested the scale of 25 000 persons. [Ukrainian activisits estimated](https://euromaidanpress.com/2022/08/30/87000-killed-civilians-documented-in-occupied-mariupol-volunteer/) the death toll to be at 87 000.</t>
   </si>
 </sst>
 </file>
@@ -183,23 +149,18 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -506,10 +467,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B20"/>
+  <dimension ref="A1:B12"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -521,150 +482,99 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>35</v>
+        <v>1</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" ht="66" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" ht="92.4" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" ht="39.6" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="184.8" x14ac:dyDescent="0.25">
+      <c r="A4" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="B4" s="4" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" ht="66" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="B5" s="4" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" ht="39.6" x14ac:dyDescent="0.25">
-      <c r="A6" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="B6" s="4" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" ht="52.8" x14ac:dyDescent="0.25">
-      <c r="A7" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="B7" s="4" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" ht="66" x14ac:dyDescent="0.25">
-      <c r="A8" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="B8" s="4" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" ht="66" x14ac:dyDescent="0.25">
-      <c r="A9" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="B9" s="4" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" ht="79.2" x14ac:dyDescent="0.25">
-      <c r="A10" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="B10" s="4" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" ht="52.8" x14ac:dyDescent="0.25">
-      <c r="A11" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="B11" s="4" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" ht="52.8" x14ac:dyDescent="0.25">
-      <c r="A12" s="2" t="s">
-        <v>26</v>
-      </c>
       <c r="B12" s="4" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" ht="52.8" x14ac:dyDescent="0.25">
-      <c r="A13" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="B13" s="4" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" ht="105.6" x14ac:dyDescent="0.25">
-      <c r="A14" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="B14" s="4" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" ht="79.2" x14ac:dyDescent="0.25">
-      <c r="A15" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="B15" s="4" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" ht="39.6" x14ac:dyDescent="0.25">
-      <c r="A16" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="B16" s="4" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" ht="118.8" x14ac:dyDescent="0.25">
-      <c r="A17" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="B17" s="4" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" ht="118.8" x14ac:dyDescent="0.25">
-      <c r="A18" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="B18" s="5" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B20" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>

</xml_diff>